<commit_message>
fixed mapping for general measurements
</commit_message>
<xml_diff>
--- a/Mappings/GeneralMeasurement - STU3.xlsx
+++ b/Mappings/GeneralMeasurement - STU3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Nictiz-STU3-Zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADB88585-DBA9-4C84-839B-11902575AE9D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0D4D5B9F-4218-4FFC-801A-8D42C3B5A67C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="159">
   <si>
     <t>Subject</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Constraints</t>
-  </si>
-  <si>
     <t>GeneralMeasurement</t>
   </si>
   <si>
@@ -481,6 +478,33 @@
   </si>
   <si>
     <t>The user may copy, distribute and pass on the information in this Health and Care Information Model under the conditions that apply for Creative Commons license Attribution-NonCommercial-ShareAlike 3.0 Netherlands (CC BY-NCSA-3.0). The content is available under Creative Commons Attribution-NonCommercial-ShareAlike 3.0 (see also http://creativecommons.org/licenses/by-nc-sa/3.0/nl/)</t>
+  </si>
+  <si>
+    <t>Maps To</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>Observation.code / Observation.component.code</t>
+  </si>
+  <si>
+    <t>Observation.status</t>
+  </si>
+  <si>
+    <t>Observation.comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation.code </t>
+  </si>
+  <si>
+    <t>Observation.method</t>
+  </si>
+  <si>
+    <t>Observation.effectiveDateTime</t>
+  </si>
+  <si>
+    <t>Observation.value/ Observation.component.value</t>
   </si>
 </sst>
 </file>
@@ -516,7 +540,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,8 +567,20 @@
         <fgColor rgb="FFD3D3D3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -604,11 +640,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -665,6 +712,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1111,7 +1166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1220,10 +1277,11 @@
     <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <ignoredErrors>
     <ignoredError sqref="C3:C8" numberStoredAsText="1"/>
   </ignoredErrors>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1447,9 +1505,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:P11"/>
+  <dimension ref="B2:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1462,10 +1522,11 @@
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>54</v>
       </c>
@@ -1499,12 +1560,15 @@
         <v>65</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B3" s="9" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -1512,278 +1576,301 @@
       <c r="F3" s="10"/>
       <c r="G3" s="11"/>
       <c r="H3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="Q3" s="22"/>
+    </row>
+    <row r="4" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="14"/>
       <c r="H4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q4" s="21"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="14"/>
       <c r="H5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5" s="21"/>
+    </row>
+    <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="14"/>
       <c r="H6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="P6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q6" s="21"/>
+    </row>
+    <row r="7" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
       <c r="C7" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
       <c r="H7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="21"/>
+    </row>
+    <row r="8" spans="2:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="14"/>
       <c r="H8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q8" s="21"/>
+    </row>
+    <row r="9" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="14"/>
       <c r="H9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q9" s="21"/>
+    </row>
+    <row r="10" spans="2:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="14"/>
       <c r="H10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q10" s="21"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
       <c r="H11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="P11" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q11" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1793,6 +1880,7 @@
     <hyperlink ref="O10" location="MeasuringMethodCodelist!A1" display="MeasuringMethodCodelist" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="J3:J10" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -1814,33 +1902,33 @@
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C3" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1870,33 +1958,33 @@
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C3" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1915,7 +2003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1928,27 +2018,27 @@
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C3" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>121</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>1</v>
@@ -1956,36 +2046,36 @@
     </row>
     <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -1993,50 +2083,50 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2066,33 +2156,33 @@
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C3" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2120,32 +2210,32 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>